<commit_message>
Final changes in figures, scrips and data
</commit_message>
<xml_diff>
--- a/data/meta_regression/yield/out1_est_wi.xlsx
+++ b/data/meta_regression/yield/out1_est_wi.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t xml:space="preserve">var</t>
   </si>
@@ -113,15 +113,12 @@
     <t xml:space="preserve">stn_scaled</t>
   </si>
   <si>
-    <t xml:space="preserve">crop</t>
+    <t xml:space="preserve">crop1</t>
   </si>
   <si>
     <t xml:space="preserve">apple</t>
   </si>
   <si>
-    <t xml:space="preserve">barley</t>
-  </si>
-  <si>
     <t xml:space="preserve">beans</t>
   </si>
   <si>
@@ -141,12 +138,6 @@
   </si>
   <si>
     <t xml:space="preserve">maize</t>
-  </si>
-  <si>
-    <t xml:space="preserve">millet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oats</t>
   </si>
   <si>
     <t xml:space="preserve">pea</t>
@@ -578,19 +569,19 @@
         <v>8</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.065</v>
+        <v>-0.014</v>
       </c>
       <c r="D2" t="n">
-        <v>0.048</v>
+        <v>0.049</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.16</v>
+        <v>-0.111</v>
       </c>
       <c r="F2" t="n">
-        <v>0.029</v>
+        <v>0.083</v>
       </c>
       <c r="G2" t="n">
-        <v>0.175</v>
+        <v>0.775</v>
       </c>
     </row>
     <row r="3">
@@ -601,16 +592,16 @@
         <v>8</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.188</v>
+        <v>-0.197</v>
       </c>
       <c r="D3" t="n">
-        <v>0.05</v>
+        <v>0.052</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.286</v>
+        <v>-0.298</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.09</v>
+        <v>-0.096</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -624,16 +615,16 @@
         <v>11</v>
       </c>
       <c r="C4" t="n">
-        <v>1.892</v>
+        <v>1.94</v>
       </c>
       <c r="D4" t="n">
-        <v>0.179</v>
+        <v>0.183</v>
       </c>
       <c r="E4" t="n">
-        <v>1.542</v>
+        <v>1.582</v>
       </c>
       <c r="F4" t="n">
-        <v>2.242</v>
+        <v>2.299</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -647,19 +638,19 @@
         <v>12</v>
       </c>
       <c r="C5" t="n">
-        <v>1.086</v>
+        <v>0.895</v>
       </c>
       <c r="D5" t="n">
-        <v>0.289</v>
+        <v>0.308</v>
       </c>
       <c r="E5" t="n">
-        <v>0.52</v>
+        <v>0.291</v>
       </c>
       <c r="F5" t="n">
-        <v>1.653</v>
+        <v>1.498</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>0.004</v>
       </c>
     </row>
     <row r="6">
@@ -670,16 +661,16 @@
         <v>13</v>
       </c>
       <c r="C6" t="n">
-        <v>1.408</v>
+        <v>1.449</v>
       </c>
       <c r="D6" t="n">
-        <v>0.16</v>
+        <v>0.165</v>
       </c>
       <c r="E6" t="n">
-        <v>1.094</v>
+        <v>1.127</v>
       </c>
       <c r="F6" t="n">
-        <v>1.723</v>
+        <v>1.772</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -693,16 +684,16 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>1.1</v>
+        <v>1.165</v>
       </c>
       <c r="D7" t="n">
-        <v>0.146</v>
+        <v>0.15</v>
       </c>
       <c r="E7" t="n">
-        <v>0.814</v>
+        <v>0.871</v>
       </c>
       <c r="F7" t="n">
-        <v>1.386</v>
+        <v>1.459</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -716,19 +707,19 @@
         <v>15</v>
       </c>
       <c r="C8" t="n">
-        <v>1.152</v>
+        <v>1.455</v>
       </c>
       <c r="D8" t="n">
-        <v>0.654</v>
+        <v>0.841</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.13</v>
+        <v>-0.194</v>
       </c>
       <c r="F8" t="n">
-        <v>2.435</v>
+        <v>3.104</v>
       </c>
       <c r="G8" t="n">
-        <v>0.078</v>
+        <v>0.084</v>
       </c>
     </row>
     <row r="9">
@@ -739,16 +730,16 @@
         <v>16</v>
       </c>
       <c r="C9" t="n">
-        <v>1.094</v>
+        <v>1.287</v>
       </c>
       <c r="D9" t="n">
-        <v>0.199</v>
+        <v>0.203</v>
       </c>
       <c r="E9" t="n">
-        <v>0.704</v>
+        <v>0.889</v>
       </c>
       <c r="F9" t="n">
-        <v>1.485</v>
+        <v>1.685</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -762,16 +753,16 @@
         <v>17</v>
       </c>
       <c r="C10" t="n">
-        <v>1.23</v>
+        <v>1.242</v>
       </c>
       <c r="D10" t="n">
-        <v>0.126</v>
+        <v>0.13</v>
       </c>
       <c r="E10" t="n">
-        <v>0.983</v>
+        <v>0.988</v>
       </c>
       <c r="F10" t="n">
-        <v>1.477</v>
+        <v>1.497</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
@@ -785,19 +776,19 @@
         <v>18</v>
       </c>
       <c r="C11" t="n">
-        <v>0.498</v>
+        <v>0.549</v>
       </c>
       <c r="D11" t="n">
-        <v>0.186</v>
+        <v>0.191</v>
       </c>
       <c r="E11" t="n">
-        <v>0.133</v>
+        <v>0.174</v>
       </c>
       <c r="F11" t="n">
-        <v>0.863</v>
+        <v>0.924</v>
       </c>
       <c r="G11" t="n">
-        <v>0.007</v>
+        <v>0.004</v>
       </c>
     </row>
     <row r="12">
@@ -808,16 +799,16 @@
         <v>19</v>
       </c>
       <c r="C12" t="n">
-        <v>1.411</v>
+        <v>1.521</v>
       </c>
       <c r="D12" t="n">
-        <v>0.302</v>
+        <v>0.308</v>
       </c>
       <c r="E12" t="n">
-        <v>0.82</v>
+        <v>0.916</v>
       </c>
       <c r="F12" t="n">
-        <v>2.003</v>
+        <v>2.125</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
@@ -831,16 +822,16 @@
         <v>20</v>
       </c>
       <c r="C13" t="n">
-        <v>1.267</v>
+        <v>1.278</v>
       </c>
       <c r="D13" t="n">
-        <v>0.162</v>
+        <v>0.166</v>
       </c>
       <c r="E13" t="n">
-        <v>0.95</v>
+        <v>0.952</v>
       </c>
       <c r="F13" t="n">
-        <v>1.584</v>
+        <v>1.604</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
@@ -854,16 +845,16 @@
         <v>21</v>
       </c>
       <c r="C14" t="n">
-        <v>0.966</v>
+        <v>1.013</v>
       </c>
       <c r="D14" t="n">
-        <v>0.089</v>
+        <v>0.092</v>
       </c>
       <c r="E14" t="n">
-        <v>0.791</v>
+        <v>0.833</v>
       </c>
       <c r="F14" t="n">
-        <v>1.142</v>
+        <v>1.194</v>
       </c>
       <c r="G14" t="n">
         <v>0</v>
@@ -877,19 +868,19 @@
         <v>8</v>
       </c>
       <c r="C15" t="n">
-        <v>0.143</v>
+        <v>0.061</v>
       </c>
       <c r="D15" t="n">
-        <v>0.053</v>
+        <v>0.054</v>
       </c>
       <c r="E15" t="n">
-        <v>0.04</v>
+        <v>-0.045</v>
       </c>
       <c r="F15" t="n">
-        <v>0.247</v>
+        <v>0.167</v>
       </c>
       <c r="G15" t="n">
-        <v>0.007</v>
+        <v>0.258</v>
       </c>
     </row>
     <row r="16">
@@ -900,19 +891,19 @@
         <v>8</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.119</v>
+        <v>-0.038</v>
       </c>
       <c r="D16" t="n">
-        <v>0.05</v>
+        <v>0.051</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.217</v>
+        <v>-0.139</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.022</v>
+        <v>0.063</v>
       </c>
       <c r="G16" t="n">
-        <v>0.017</v>
+        <v>0.458</v>
       </c>
     </row>
     <row r="17">
@@ -923,16 +914,16 @@
         <v>25</v>
       </c>
       <c r="C17" t="n">
-        <v>0.605</v>
+        <v>0.65</v>
       </c>
       <c r="D17" t="n">
-        <v>0.097</v>
+        <v>0.099</v>
       </c>
       <c r="E17" t="n">
-        <v>0.416</v>
+        <v>0.456</v>
       </c>
       <c r="F17" t="n">
-        <v>0.794</v>
+        <v>0.844</v>
       </c>
       <c r="G17" t="n">
         <v>0</v>
@@ -946,16 +937,16 @@
         <v>26</v>
       </c>
       <c r="C18" t="n">
-        <v>1.646</v>
+        <v>1.742</v>
       </c>
       <c r="D18" t="n">
-        <v>0.125</v>
+        <v>0.127</v>
       </c>
       <c r="E18" t="n">
-        <v>1.401</v>
+        <v>1.492</v>
       </c>
       <c r="F18" t="n">
-        <v>1.89</v>
+        <v>1.991</v>
       </c>
       <c r="G18" t="n">
         <v>0</v>
@@ -969,16 +960,16 @@
         <v>27</v>
       </c>
       <c r="C19" t="n">
-        <v>1.73</v>
+        <v>1.791</v>
       </c>
       <c r="D19" t="n">
-        <v>0.12</v>
+        <v>0.122</v>
       </c>
       <c r="E19" t="n">
-        <v>1.495</v>
+        <v>1.551</v>
       </c>
       <c r="F19" t="n">
-        <v>1.966</v>
+        <v>2.031</v>
       </c>
       <c r="G19" t="n">
         <v>0</v>
@@ -992,16 +983,16 @@
         <v>28</v>
       </c>
       <c r="C20" t="n">
-        <v>1.107</v>
+        <v>1.057</v>
       </c>
       <c r="D20" t="n">
-        <v>0.112</v>
+        <v>0.069</v>
       </c>
       <c r="E20" t="n">
-        <v>0.888</v>
+        <v>0.923</v>
       </c>
       <c r="F20" t="n">
-        <v>1.326</v>
+        <v>1.191</v>
       </c>
       <c r="G20" t="n">
         <v>0</v>
@@ -1009,22 +1000,22 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C21" t="n">
-        <v>1.006</v>
+        <v>0.202</v>
       </c>
       <c r="D21" t="n">
-        <v>0.083</v>
+        <v>0.053</v>
       </c>
       <c r="E21" t="n">
-        <v>0.844</v>
+        <v>0.099</v>
       </c>
       <c r="F21" t="n">
-        <v>1.168</v>
+        <v>0.305</v>
       </c>
       <c r="G21" t="n">
         <v>0</v>
@@ -1032,94 +1023,94 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
       </c>
       <c r="C22" t="n">
-        <v>0.095</v>
+        <v>0.241</v>
       </c>
       <c r="D22" t="n">
-        <v>0.051</v>
+        <v>0.052</v>
       </c>
       <c r="E22" t="n">
-        <v>-0.006</v>
+        <v>0.139</v>
       </c>
       <c r="F22" t="n">
-        <v>0.195</v>
+        <v>0.344</v>
       </c>
       <c r="G22" t="n">
-        <v>0.065</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B23" t="s">
         <v>8</v>
       </c>
       <c r="C23" t="n">
-        <v>0.206</v>
+        <v>0.011</v>
       </c>
       <c r="D23" t="n">
-        <v>0.051</v>
+        <v>0.061</v>
       </c>
       <c r="E23" t="n">
-        <v>0.106</v>
+        <v>-0.109</v>
       </c>
       <c r="F23" t="n">
-        <v>0.305</v>
+        <v>0.131</v>
       </c>
       <c r="G23" t="n">
-        <v>0</v>
+        <v>0.854</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
         <v>8</v>
       </c>
       <c r="C24" t="n">
-        <v>0.143</v>
+        <v>0.002</v>
       </c>
       <c r="D24" t="n">
-        <v>0.056</v>
+        <v>0.051</v>
       </c>
       <c r="E24" t="n">
-        <v>0.033</v>
+        <v>-0.099</v>
       </c>
       <c r="F24" t="n">
-        <v>0.253</v>
+        <v>0.102</v>
       </c>
       <c r="G24" t="n">
-        <v>0.011</v>
+        <v>0.976</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="C25" t="n">
-        <v>0.015</v>
+        <v>1.17</v>
       </c>
       <c r="D25" t="n">
-        <v>0.05</v>
+        <v>0.366</v>
       </c>
       <c r="E25" t="n">
-        <v>-0.082</v>
+        <v>0.453</v>
       </c>
       <c r="F25" t="n">
-        <v>0.113</v>
+        <v>1.887</v>
       </c>
       <c r="G25" t="n">
-        <v>0.755</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="26">
@@ -1127,22 +1118,22 @@
         <v>33</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C26" t="n">
-        <v>1.167</v>
+        <v>2.235</v>
       </c>
       <c r="D26" t="n">
-        <v>0.354</v>
+        <v>0.423</v>
       </c>
       <c r="E26" t="n">
-        <v>0.473</v>
+        <v>1.406</v>
       </c>
       <c r="F26" t="n">
-        <v>1.86</v>
+        <v>3.064</v>
       </c>
       <c r="G26" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -1150,22 +1141,22 @@
         <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C27" t="n">
-        <v>0.318</v>
+        <v>1.899</v>
       </c>
       <c r="D27" t="n">
-        <v>0.911</v>
+        <v>0.525</v>
       </c>
       <c r="E27" t="n">
-        <v>-1.468</v>
+        <v>0.871</v>
       </c>
       <c r="F27" t="n">
-        <v>2.104</v>
+        <v>2.928</v>
       </c>
       <c r="G27" t="n">
-        <v>0.727</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -1173,22 +1164,22 @@
         <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C28" t="n">
-        <v>2.199</v>
+        <v>1.483</v>
       </c>
       <c r="D28" t="n">
-        <v>0.412</v>
+        <v>0.569</v>
       </c>
       <c r="E28" t="n">
-        <v>1.392</v>
+        <v>0.368</v>
       </c>
       <c r="F28" t="n">
-        <v>3.006</v>
+        <v>2.597</v>
       </c>
       <c r="G28" t="n">
-        <v>0</v>
+        <v>0.009</v>
       </c>
     </row>
     <row r="29">
@@ -1196,22 +1187,22 @@
         <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C29" t="n">
-        <v>1.898</v>
+        <v>1.799</v>
       </c>
       <c r="D29" t="n">
-        <v>0.51</v>
+        <v>0.686</v>
       </c>
       <c r="E29" t="n">
-        <v>0.899</v>
+        <v>0.455</v>
       </c>
       <c r="F29" t="n">
-        <v>2.897</v>
+        <v>3.144</v>
       </c>
       <c r="G29" t="n">
-        <v>0</v>
+        <v>0.009</v>
       </c>
     </row>
     <row r="30">
@@ -1219,22 +1210,22 @@
         <v>33</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C30" t="n">
-        <v>1.476</v>
+        <v>1.37</v>
       </c>
       <c r="D30" t="n">
-        <v>0.551</v>
+        <v>0.553</v>
       </c>
       <c r="E30" t="n">
-        <v>0.395</v>
+        <v>0.286</v>
       </c>
       <c r="F30" t="n">
-        <v>2.557</v>
+        <v>2.454</v>
       </c>
       <c r="G30" t="n">
-        <v>0.007</v>
+        <v>0.013</v>
       </c>
     </row>
     <row r="31">
@@ -1242,22 +1233,22 @@
         <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C31" t="n">
-        <v>1.788</v>
+        <v>0.749</v>
       </c>
       <c r="D31" t="n">
-        <v>0.666</v>
+        <v>0.61</v>
       </c>
       <c r="E31" t="n">
-        <v>0.482</v>
+        <v>-0.447</v>
       </c>
       <c r="F31" t="n">
-        <v>3.094</v>
+        <v>1.944</v>
       </c>
       <c r="G31" t="n">
-        <v>0.007</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="32">
@@ -1265,22 +1256,22 @@
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C32" t="n">
-        <v>1.37</v>
+        <v>1.381</v>
       </c>
       <c r="D32" t="n">
-        <v>0.536</v>
+        <v>0.1</v>
       </c>
       <c r="E32" t="n">
-        <v>0.32</v>
+        <v>1.185</v>
       </c>
       <c r="F32" t="n">
-        <v>2.42</v>
+        <v>1.576</v>
       </c>
       <c r="G32" t="n">
-        <v>0.011</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -1288,22 +1279,22 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C33" t="n">
-        <v>0.748</v>
+        <v>2.306</v>
       </c>
       <c r="D33" t="n">
-        <v>0.589</v>
+        <v>0.618</v>
       </c>
       <c r="E33" t="n">
-        <v>-0.406</v>
+        <v>1.094</v>
       </c>
       <c r="F33" t="n">
-        <v>1.902</v>
+        <v>3.517</v>
       </c>
       <c r="G33" t="n">
-        <v>0.204</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -1311,19 +1302,19 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C34" t="n">
-        <v>1.348</v>
+        <v>1.387</v>
       </c>
       <c r="D34" t="n">
-        <v>0.096</v>
+        <v>0.396</v>
       </c>
       <c r="E34" t="n">
-        <v>1.16</v>
+        <v>0.611</v>
       </c>
       <c r="F34" t="n">
-        <v>1.537</v>
+        <v>2.162</v>
       </c>
       <c r="G34" t="n">
         <v>0</v>
@@ -1334,22 +1325,22 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C35" t="n">
-        <v>0.727</v>
+        <v>1.784</v>
       </c>
       <c r="D35" t="n">
-        <v>0.518</v>
+        <v>0.512</v>
       </c>
       <c r="E35" t="n">
-        <v>-0.287</v>
+        <v>0.779</v>
       </c>
       <c r="F35" t="n">
-        <v>1.742</v>
+        <v>2.788</v>
       </c>
       <c r="G35" t="n">
-        <v>0.16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -1357,22 +1348,22 @@
         <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C36" t="n">
-        <v>2.242</v>
+        <v>2.173</v>
       </c>
       <c r="D36" t="n">
-        <v>0.792</v>
+        <v>0.312</v>
       </c>
       <c r="E36" t="n">
-        <v>0.69</v>
+        <v>1.561</v>
       </c>
       <c r="F36" t="n">
-        <v>3.793</v>
+        <v>2.784</v>
       </c>
       <c r="G36" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -1380,19 +1371,19 @@
         <v>33</v>
       </c>
       <c r="B37" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C37" t="n">
-        <v>2.609</v>
+        <v>0.87</v>
       </c>
       <c r="D37" t="n">
-        <v>0.721</v>
+        <v>0.064</v>
       </c>
       <c r="E37" t="n">
-        <v>1.196</v>
+        <v>0.746</v>
       </c>
       <c r="F37" t="n">
-        <v>4.022</v>
+        <v>0.995</v>
       </c>
       <c r="G37" t="n">
         <v>0</v>
@@ -1403,22 +1394,22 @@
         <v>33</v>
       </c>
       <c r="B38" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C38" t="n">
-        <v>1.362</v>
+        <v>-0.04</v>
       </c>
       <c r="D38" t="n">
-        <v>0.384</v>
+        <v>0.29</v>
       </c>
       <c r="E38" t="n">
-        <v>0.61</v>
+        <v>-0.608</v>
       </c>
       <c r="F38" t="n">
-        <v>2.114</v>
+        <v>0.529</v>
       </c>
       <c r="G38" t="n">
-        <v>0</v>
+        <v>0.891</v>
       </c>
     </row>
     <row r="39">
@@ -1426,22 +1417,22 @@
         <v>33</v>
       </c>
       <c r="B39" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C39" t="n">
-        <v>0.492</v>
+        <v>2.754</v>
       </c>
       <c r="D39" t="n">
-        <v>0.527</v>
+        <v>0.308</v>
       </c>
       <c r="E39" t="n">
-        <v>-0.541</v>
+        <v>2.15</v>
       </c>
       <c r="F39" t="n">
-        <v>1.525</v>
+        <v>3.358</v>
       </c>
       <c r="G39" t="n">
-        <v>0.351</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -1449,19 +1440,19 @@
         <v>33</v>
       </c>
       <c r="B40" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C40" t="n">
-        <v>2.158</v>
+        <v>1.746</v>
       </c>
       <c r="D40" t="n">
-        <v>0.304</v>
+        <v>0.171</v>
       </c>
       <c r="E40" t="n">
-        <v>1.563</v>
+        <v>1.411</v>
       </c>
       <c r="F40" t="n">
-        <v>2.754</v>
+        <v>2.081</v>
       </c>
       <c r="G40" t="n">
         <v>0</v>
@@ -1469,91 +1460,91 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="B41" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C41" t="n">
-        <v>0.833</v>
+        <v>1.176</v>
       </c>
       <c r="D41" t="n">
-        <v>0.062</v>
+        <v>0.389</v>
       </c>
       <c r="E41" t="n">
-        <v>0.712</v>
+        <v>0.414</v>
       </c>
       <c r="F41" t="n">
-        <v>0.954</v>
+        <v>1.938</v>
       </c>
       <c r="G41" t="n">
-        <v>0</v>
+        <v>0.002</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="B42" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C42" t="n">
-        <v>-0.507</v>
+        <v>1.076</v>
       </c>
       <c r="D42" t="n">
-        <v>0.336</v>
+        <v>0.054</v>
       </c>
       <c r="E42" t="n">
-        <v>-1.167</v>
+        <v>0.971</v>
       </c>
       <c r="F42" t="n">
-        <v>0.152</v>
+        <v>1.181</v>
       </c>
       <c r="G42" t="n">
-        <v>0.132</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="B43" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C43" t="n">
-        <v>2.73</v>
+        <v>1.494</v>
       </c>
       <c r="D43" t="n">
-        <v>0.301</v>
+        <v>0.603</v>
       </c>
       <c r="E43" t="n">
-        <v>2.141</v>
+        <v>0.313</v>
       </c>
       <c r="F43" t="n">
-        <v>3.32</v>
+        <v>2.675</v>
       </c>
       <c r="G43" t="n">
-        <v>0</v>
+        <v>0.013</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="B44" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C44" t="n">
-        <v>1.73</v>
+        <v>1.923</v>
       </c>
       <c r="D44" t="n">
-        <v>0.169</v>
+        <v>0.276</v>
       </c>
       <c r="E44" t="n">
-        <v>1.399</v>
+        <v>1.382</v>
       </c>
       <c r="F44" t="n">
-        <v>2.06</v>
+        <v>2.464</v>
       </c>
       <c r="G44" t="n">
         <v>0</v>
@@ -1561,45 +1552,45 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B45" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C45" t="n">
-        <v>1.173</v>
+        <v>1.902</v>
       </c>
       <c r="D45" t="n">
-        <v>0.377</v>
+        <v>0.554</v>
       </c>
       <c r="E45" t="n">
-        <v>0.433</v>
+        <v>0.817</v>
       </c>
       <c r="F45" t="n">
-        <v>1.913</v>
+        <v>2.987</v>
       </c>
       <c r="G45" t="n">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B46" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C46" t="n">
-        <v>1.04</v>
+        <v>2.198</v>
       </c>
       <c r="D46" t="n">
-        <v>0.052</v>
+        <v>0.328</v>
       </c>
       <c r="E46" t="n">
-        <v>0.938</v>
+        <v>1.555</v>
       </c>
       <c r="F46" t="n">
-        <v>1.142</v>
+        <v>2.841</v>
       </c>
       <c r="G46" t="n">
         <v>0</v>
@@ -1607,91 +1598,91 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B47" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C47" t="n">
-        <v>1.489</v>
+        <v>2.114</v>
       </c>
       <c r="D47" t="n">
-        <v>0.586</v>
+        <v>0.222</v>
       </c>
       <c r="E47" t="n">
-        <v>0.34</v>
+        <v>1.678</v>
       </c>
       <c r="F47" t="n">
-        <v>2.637</v>
+        <v>2.55</v>
       </c>
       <c r="G47" t="n">
-        <v>0.011</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B48" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="C48" t="n">
-        <v>1.917</v>
+        <v>0.101</v>
       </c>
       <c r="D48" t="n">
-        <v>0.277</v>
+        <v>0.049</v>
       </c>
       <c r="E48" t="n">
-        <v>1.375</v>
+        <v>0.004</v>
       </c>
       <c r="F48" t="n">
-        <v>2.459</v>
+        <v>0.198</v>
       </c>
       <c r="G48" t="n">
-        <v>0</v>
+        <v>0.041</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B49" t="s">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="C49" t="n">
-        <v>1.901</v>
+        <v>0.076</v>
       </c>
       <c r="D49" t="n">
-        <v>0.539</v>
+        <v>0.051</v>
       </c>
       <c r="E49" t="n">
-        <v>0.843</v>
+        <v>-0.024</v>
       </c>
       <c r="F49" t="n">
-        <v>2.958</v>
+        <v>0.175</v>
       </c>
       <c r="G49" t="n">
-        <v>0</v>
+        <v>0.137</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B50" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="C50" t="n">
-        <v>2.186</v>
+        <v>0.362</v>
       </c>
       <c r="D50" t="n">
-        <v>0.32</v>
+        <v>0.054</v>
       </c>
       <c r="E50" t="n">
-        <v>1.558</v>
+        <v>0.256</v>
       </c>
       <c r="F50" t="n">
-        <v>2.814</v>
+        <v>0.469</v>
       </c>
       <c r="G50" t="n">
         <v>0</v>
@@ -1699,186 +1690,94 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B51" t="s">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="C51" t="n">
-        <v>1.887</v>
+        <v>0.013</v>
       </c>
       <c r="D51" t="n">
-        <v>0.219</v>
+        <v>0.053</v>
       </c>
       <c r="E51" t="n">
-        <v>1.458</v>
+        <v>-0.09</v>
       </c>
       <c r="F51" t="n">
-        <v>2.317</v>
+        <v>0.116</v>
       </c>
       <c r="G51" t="n">
-        <v>0</v>
+        <v>0.801</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B52" t="s">
         <v>8</v>
       </c>
       <c r="C52" t="n">
-        <v>0.111</v>
+        <v>-0.037</v>
       </c>
       <c r="D52" t="n">
-        <v>0.048</v>
+        <v>0.055</v>
       </c>
       <c r="E52" t="n">
-        <v>0.017</v>
+        <v>-0.145</v>
       </c>
       <c r="F52" t="n">
-        <v>0.205</v>
+        <v>0.071</v>
       </c>
       <c r="G52" t="n">
-        <v>0.02</v>
+        <v>0.506</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B53" t="s">
         <v>8</v>
       </c>
       <c r="C53" t="n">
-        <v>0.084</v>
+        <v>0.021</v>
       </c>
       <c r="D53" t="n">
-        <v>0.049</v>
+        <v>0.058</v>
       </c>
       <c r="E53" t="n">
-        <v>-0.013</v>
+        <v>-0.094</v>
       </c>
       <c r="F53" t="n">
-        <v>0.18</v>
+        <v>0.136</v>
       </c>
       <c r="G53" t="n">
-        <v>0.09</v>
+        <v>0.719</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B54" t="s">
         <v>8</v>
       </c>
       <c r="C54" t="n">
-        <v>0.348</v>
+        <v>0.11</v>
       </c>
       <c r="D54" t="n">
+        <v>0.057</v>
+      </c>
+      <c r="E54" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0.221</v>
+      </c>
+      <c r="G54" t="n">
         <v>0.053</v>
-      </c>
-      <c r="E54" t="n">
-        <v>0.244</v>
-      </c>
-      <c r="F54" t="n">
-        <v>0.452</v>
-      </c>
-      <c r="G54" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="s">
-        <v>64</v>
-      </c>
-      <c r="B55" t="s">
-        <v>8</v>
-      </c>
-      <c r="C55" t="n">
-        <v>0.058</v>
-      </c>
-      <c r="D55" t="n">
-        <v>0.051</v>
-      </c>
-      <c r="E55" t="n">
-        <v>-0.042</v>
-      </c>
-      <c r="F55" t="n">
-        <v>0.159</v>
-      </c>
-      <c r="G55" t="n">
-        <v>0.253</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="s">
-        <v>65</v>
-      </c>
-      <c r="B56" t="s">
-        <v>8</v>
-      </c>
-      <c r="C56" t="n">
-        <v>0.035</v>
-      </c>
-      <c r="D56" t="n">
-        <v>0.054</v>
-      </c>
-      <c r="E56" t="n">
-        <v>-0.07</v>
-      </c>
-      <c r="F56" t="n">
-        <v>0.141</v>
-      </c>
-      <c r="G56" t="n">
-        <v>0.509</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="s">
-        <v>66</v>
-      </c>
-      <c r="B57" t="s">
-        <v>8</v>
-      </c>
-      <c r="C57" t="n">
-        <v>-0.076</v>
-      </c>
-      <c r="D57" t="n">
-        <v>0.054</v>
-      </c>
-      <c r="E57" t="n">
-        <v>-0.183</v>
-      </c>
-      <c r="F57" t="n">
-        <v>0.031</v>
-      </c>
-      <c r="G57" t="n">
-        <v>0.162</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="s">
-        <v>67</v>
-      </c>
-      <c r="B58" t="s">
-        <v>8</v>
-      </c>
-      <c r="C58" t="n">
-        <v>0.084</v>
-      </c>
-      <c r="D58" t="n">
-        <v>0.056</v>
-      </c>
-      <c r="E58" t="n">
-        <v>-0.025</v>
-      </c>
-      <c r="F58" t="n">
-        <v>0.193</v>
-      </c>
-      <c r="G58" t="n">
-        <v>0.131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>